<commit_message>
finilised feature subset, comments added
</commit_message>
<xml_diff>
--- a/DIAS Attributes - Values 2017_eks.xlsx
+++ b/DIAS Attributes - Values 2017_eks.xlsx
@@ -17,14 +17,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$F$2:$F$2260</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$F$2:$G$2260</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3396" uniqueCount="1231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3396" uniqueCount="1232">
   <si>
     <t>AGER_TYP</t>
   </si>
@@ -3716,14 +3716,17 @@
     <t>Type2</t>
   </si>
   <si>
-    <t>'MIN_GEBAEUDEJAHR'</t>
+    <t>ANZ_KINDER</t>
+  </si>
+  <si>
+    <t>categorical_mixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3756,12 +3759,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -3999,7 +3996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4106,7 +4103,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4413,8 +4409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G2260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B89" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A2145" workbookViewId="0">
+      <selection activeCell="B2093" sqref="B2093"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4874,7 +4870,7 @@
       </c>
     </row>
     <row r="41" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="33" t="s">
         <v>1230</v>
       </c>
       <c r="C41" s="10" t="s">
@@ -4919,6 +4915,9 @@
       </c>
       <c r="E43" s="5" t="s">
         <v>251</v>
+      </c>
+      <c r="F43" s="52" t="s">
+        <v>1222</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.3">
@@ -26292,9 +26291,7 @@
       <c r="F1979" s="52" t="s">
         <v>1222</v>
       </c>
-      <c r="G1979" s="52" t="s">
-        <v>1224</v>
-      </c>
+      <c r="G1979" s="52"/>
     </row>
     <row r="1980" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B1980" s="36"/>
@@ -26975,7 +26972,7 @@
         <v>679</v>
       </c>
       <c r="F2040" s="52" t="s">
-        <v>1225</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="2041" spans="2:6" x14ac:dyDescent="0.3">
@@ -29397,7 +29394,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F2:F2260"/>
+  <autoFilter ref="F2:G2260"/>
   <mergeCells count="7">
     <mergeCell ref="E1986:E1987"/>
     <mergeCell ref="E1908:E1910"/>
@@ -29437,15 +29434,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101004F7AABC398522B40A32DAEEC36E85685" ma:contentTypeVersion="0" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fcd56fbdc9ca50fa66f2b7c9cf7a93ad">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="246f02dd96380beb4f7cdcce14d77fd6">
     <xsd:element name="properties">
@@ -29494,6 +29482,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -29501,14 +29498,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3EA3FA-F7A9-4EB1-BDA9-02346FC3DB01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BABB9296-97A3-46A1-A889-43BF8783A394}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -29519,6 +29508,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3EA3FA-F7A9-4EB1-BDA9-02346FC3DB01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>